<commit_message>
Established Working Serial Comms with Arduino
</commit_message>
<xml_diff>
--- a/electrical_hardware/APWCR_Electrical_Pin_Connections.xlsx
+++ b/electrical_hardware/APWCR_Electrical_Pin_Connections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\UT_Files\Senior_Design_Repos\APWCR_Software\electrical_hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720607D7-A0CB-4229-9515-6D9E7B79FB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8E3E6B-DC21-4ACA-80B5-31AF7D02D4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Layout" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="113">
   <si>
     <t>12V Power Distribution Rail</t>
   </si>
@@ -338,6 +338,33 @@
   </si>
   <si>
     <t>MG996R Servos</t>
+  </si>
+  <si>
+    <t>5V+ Servo PDB</t>
+  </si>
+  <si>
+    <t>5V- Servo PDB</t>
+  </si>
+  <si>
+    <t>5V+ Aux PDB</t>
+  </si>
+  <si>
+    <t>5V- Aux PDB</t>
+  </si>
+  <si>
+    <t>Aux Rail Ground</t>
+  </si>
+  <si>
+    <t>Servo Rail Ground</t>
+  </si>
+  <si>
+    <t>Arduino GND</t>
+  </si>
+  <si>
+    <t>HC-SR04 GND</t>
+  </si>
+  <si>
+    <t>HC-SR04 VCC</t>
   </si>
 </sst>
 </file>
@@ -512,7 +539,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -859,11 +886,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -882,9 +935,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -898,31 +948,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -975,6 +1000,68 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -984,6 +1071,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -993,38 +1089,15 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1307,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S25"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1320,26 +1393,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
+      <c r="S2" s="86"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B3" s="9"/>
@@ -1361,22 +1434,28 @@
       <c r="R3" s="10"/>
       <c r="S3" s="11"/>
     </row>
-    <row r="4" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:19" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
+      <c r="E4" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="69" t="s">
+        <v>110</v>
+      </c>
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
       <c r="S4" s="14"/>
@@ -1385,40 +1464,40 @@
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="M5" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="18" t="s">
+      <c r="N5" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="18" t="s">
+      <c r="O5" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="58" t="s">
         <v>24</v>
       </c>
       <c r="Q5" s="11"/>
@@ -1427,27 +1506,27 @@
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B6" s="12"/>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="75" t="s">
+      <c r="E6" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="75"/>
-      <c r="Q6" s="20" t="s">
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="84"/>
+      <c r="P6" s="84"/>
+      <c r="Q6" s="19" t="s">
         <v>25</v>
       </c>
       <c r="R6" s="13"/>
@@ -1455,25 +1534,25 @@
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B7" s="12"/>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="75"/>
-      <c r="M7" s="75"/>
-      <c r="N7" s="75"/>
-      <c r="O7" s="75"/>
-      <c r="P7" s="75"/>
-      <c r="Q7" s="20" t="s">
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
+      <c r="L7" s="84"/>
+      <c r="M7" s="84"/>
+      <c r="N7" s="84"/>
+      <c r="O7" s="84"/>
+      <c r="P7" s="84"/>
+      <c r="Q7" s="19" t="s">
         <v>26</v>
       </c>
       <c r="R7" s="13"/>
@@ -1483,78 +1562,82 @@
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="15"/>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="L8" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="18" t="s">
+      <c r="N8" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="18" t="s">
+      <c r="O8" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="59" t="s">
         <v>12</v>
       </c>
       <c r="Q8" s="17"/>
       <c r="R8" s="13"/>
       <c r="S8" s="14"/>
     </row>
-    <row r="9" spans="2:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:19" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="70" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="H9" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="I9" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="J9" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="K9" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="L9" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="M9" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="N9" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="57"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
       <c r="S9" s="14"/>
@@ -1579,22 +1662,22 @@
       <c r="R10" s="13"/>
       <c r="S10" s="14"/>
     </row>
-    <row r="11" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:19" ht="29.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
       <c r="S11" s="14"/>
@@ -1603,40 +1686,40 @@
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="30" t="s">
+      <c r="I12" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="30" t="s">
+      <c r="J12" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="30" t="s">
+      <c r="K12" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="30" t="s">
+      <c r="L12" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="30" t="s">
+      <c r="M12" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="30" t="s">
+      <c r="N12" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="O12" s="30" t="s">
+      <c r="O12" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="P12" s="30" t="s">
+      <c r="P12" s="63" t="s">
         <v>24</v>
       </c>
       <c r="Q12" s="11"/>
@@ -1645,27 +1728,27 @@
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B13" s="12"/>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="76" t="s">
+      <c r="E13" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="76"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="76"/>
-      <c r="N13" s="76"/>
-      <c r="O13" s="76"/>
-      <c r="P13" s="76"/>
-      <c r="Q13" s="21" t="s">
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85"/>
+      <c r="L13" s="85"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="20" t="s">
         <v>25</v>
       </c>
       <c r="R13" s="13"/>
@@ -1673,25 +1756,25 @@
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B14" s="12"/>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="76"/>
-      <c r="L14" s="76"/>
-      <c r="M14" s="76"/>
-      <c r="N14" s="76"/>
-      <c r="O14" s="76"/>
-      <c r="P14" s="76"/>
-      <c r="Q14" s="21" t="s">
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85"/>
+      <c r="L14" s="85"/>
+      <c r="M14" s="85"/>
+      <c r="N14" s="85"/>
+      <c r="O14" s="85"/>
+      <c r="P14" s="85"/>
+      <c r="Q14" s="20" t="s">
         <v>26</v>
       </c>
       <c r="R14" s="13"/>
@@ -1701,40 +1784,40 @@
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="30" t="s">
+      <c r="I15" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="30" t="s">
+      <c r="J15" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="30" t="s">
+      <c r="K15" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="L15" s="30" t="s">
+      <c r="L15" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="30" t="s">
+      <c r="M15" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="N15" s="30" t="s">
+      <c r="N15" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="O15" s="30" t="s">
+      <c r="O15" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="P15" s="30" t="s">
+      <c r="P15" s="64" t="s">
         <v>12</v>
       </c>
       <c r="Q15" s="17"/>
@@ -1745,24 +1828,26 @@
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="31" t="s">
+      <c r="G16" s="62"/>
+      <c r="H16" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="P16" s="32" t="s">
+      <c r="P16" s="61" t="s">
         <v>42</v>
       </c>
       <c r="Q16" s="13"/>
@@ -1793,24 +1878,30 @@
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="31" t="s">
+      <c r="G18" s="67"/>
+      <c r="H18" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="N18" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="O18" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="P18" s="32" t="s">
+      <c r="P18" s="66" t="s">
         <v>48</v>
       </c>
       <c r="Q18" s="13"/>
@@ -1821,40 +1912,40 @@
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="30" t="s">
+      <c r="I19" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="30" t="s">
+      <c r="J19" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="30" t="s">
+      <c r="K19" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="30" t="s">
+      <c r="L19" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="30" t="s">
+      <c r="M19" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="N19" s="30" t="s">
+      <c r="N19" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="30" t="s">
+      <c r="O19" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="P19" s="30" t="s">
+      <c r="P19" s="63" t="s">
         <v>24</v>
       </c>
       <c r="Q19" s="11"/>
@@ -1863,27 +1954,27 @@
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B20" s="12"/>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="76" t="s">
+      <c r="E20" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="76"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="76"/>
-      <c r="M20" s="76"/>
-      <c r="N20" s="76"/>
-      <c r="O20" s="76"/>
-      <c r="P20" s="76"/>
-      <c r="Q20" s="21" t="s">
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="85"/>
+      <c r="L20" s="85"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="85"/>
+      <c r="O20" s="85"/>
+      <c r="P20" s="85"/>
+      <c r="Q20" s="20" t="s">
         <v>25</v>
       </c>
       <c r="R20" s="13"/>
@@ -1891,25 +1982,25 @@
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B21" s="12"/>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="76"/>
-      <c r="K21" s="76"/>
-      <c r="L21" s="76"/>
-      <c r="M21" s="76"/>
-      <c r="N21" s="76"/>
-      <c r="O21" s="76"/>
-      <c r="P21" s="76"/>
-      <c r="Q21" s="21" t="s">
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="85"/>
+      <c r="L21" s="85"/>
+      <c r="M21" s="85"/>
+      <c r="N21" s="85"/>
+      <c r="O21" s="85"/>
+      <c r="P21" s="85"/>
+      <c r="Q21" s="20" t="s">
         <v>26</v>
       </c>
       <c r="R21" s="13"/>
@@ -1919,40 +2010,40 @@
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="30" t="s">
+      <c r="H22" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="30" t="s">
+      <c r="I22" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="30" t="s">
+      <c r="J22" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="K22" s="30" t="s">
+      <c r="K22" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="30" t="s">
+      <c r="L22" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="30" t="s">
+      <c r="M22" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="N22" s="30" t="s">
+      <c r="N22" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="O22" s="30" t="s">
+      <c r="O22" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="P22" s="30" t="s">
+      <c r="P22" s="64" t="s">
         <v>12</v>
       </c>
       <c r="Q22" s="17"/>
@@ -1963,24 +2054,24 @@
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="31" t="s">
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="P23" s="32" t="s">
+      <c r="P23" s="61" t="s">
         <v>46</v>
       </c>
       <c r="Q23" s="13"/>
@@ -2042,10 +2133,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4C9B7A-925E-4ACB-8F3D-3CC4DA199EDA}">
-  <dimension ref="B2:AP31"/>
+  <dimension ref="B2:AP28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AN16" sqref="AN16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2059,51 +2150,51 @@
   <sheetData>
     <row r="2" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="2:42" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="65"/>
-      <c r="M3" s="63" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="77"/>
+      <c r="M3" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="65"/>
-      <c r="AB3" s="63" t="s">
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="77"/>
+      <c r="AB3" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="65"/>
-      <c r="AK3" s="52"/>
-      <c r="AL3" s="52"/>
-      <c r="AM3" s="52"/>
-      <c r="AN3" s="52"/>
-      <c r="AO3" s="52"/>
-      <c r="AP3" s="52"/>
+      <c r="AC3" s="76"/>
+      <c r="AD3" s="76"/>
+      <c r="AE3" s="76"/>
+      <c r="AF3" s="76"/>
+      <c r="AG3" s="76"/>
+      <c r="AH3" s="76"/>
+      <c r="AI3" s="76"/>
+      <c r="AJ3" s="77"/>
+      <c r="AK3" s="42"/>
+      <c r="AL3" s="42"/>
+      <c r="AM3" s="42"/>
+      <c r="AN3" s="42"/>
+      <c r="AO3" s="42"/>
+      <c r="AP3" s="42"/>
     </row>
     <row r="4" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="1"/>
@@ -2142,10 +2233,10 @@
     </row>
     <row r="5" spans="2:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="4"/>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="30" t="s">
         <v>57</v>
       </c>
       <c r="E5" s="72" t="s">
@@ -2154,90 +2245,90 @@
       <c r="F5" s="72"/>
       <c r="G5" s="72"/>
       <c r="H5" s="72"/>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="24" t="s">
         <v>59</v>
       </c>
       <c r="K5" s="5"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="50" t="s">
+      <c r="N5" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="44" t="s">
+      <c r="O5" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="66" t="s">
+      <c r="P5" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="66"/>
-      <c r="X5" s="45" t="s">
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="Y5" s="39" t="s">
+      <c r="Y5" s="29" t="s">
         <v>81</v>
       </c>
       <c r="Z5" s="5"/>
       <c r="AB5" s="4"/>
-      <c r="AC5" s="62" t="s">
+      <c r="AC5" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="AD5" s="53" t="s">
+      <c r="AD5" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="AE5" s="69" t="s">
+      <c r="AE5" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="AF5" s="69"/>
-      <c r="AG5" s="69"/>
-      <c r="AH5" s="54" t="s">
+      <c r="AF5" s="78"/>
+      <c r="AG5" s="78"/>
+      <c r="AH5" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="AI5" s="59" t="s">
+      <c r="AI5" s="49" t="s">
         <v>98</v>
       </c>
       <c r="AJ5" s="5"/>
     </row>
     <row r="6" spans="2:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B6" s="4"/>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="31" t="s">
         <v>58</v>
       </c>
       <c r="E6" s="73"/>
       <c r="F6" s="73"/>
       <c r="G6" s="73"/>
       <c r="H6" s="73"/>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="25" t="s">
         <v>60</v>
       </c>
       <c r="K6" s="5"/>
       <c r="M6" s="4"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="67"/>
-      <c r="X6" s="47"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="82"/>
+      <c r="X6" s="37"/>
       <c r="Z6" s="5"/>
       <c r="AB6" s="4"/>
-      <c r="AC6" s="61"/>
-      <c r="AD6" s="55"/>
-      <c r="AE6" s="70"/>
-      <c r="AF6" s="70"/>
-      <c r="AG6" s="70"/>
-      <c r="AH6" s="56"/>
-      <c r="AI6" s="60"/>
+      <c r="AC6" s="51"/>
+      <c r="AD6" s="45"/>
+      <c r="AE6" s="79"/>
+      <c r="AF6" s="79"/>
+      <c r="AG6" s="79"/>
+      <c r="AH6" s="46"/>
+      <c r="AI6" s="50"/>
       <c r="AJ6" s="5"/>
     </row>
     <row r="7" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -2250,61 +2341,61 @@
       <c r="I7" s="5"/>
       <c r="K7" s="5"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="51" t="s">
+      <c r="N7" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="48" t="s">
+      <c r="O7" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P7" s="68"/>
-      <c r="Q7" s="68"/>
-      <c r="R7" s="68"/>
-      <c r="S7" s="68"/>
-      <c r="T7" s="68"/>
-      <c r="U7" s="68"/>
-      <c r="V7" s="68"/>
-      <c r="W7" s="68"/>
-      <c r="X7" s="49" t="s">
+      <c r="P7" s="83"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="83"/>
+      <c r="S7" s="83"/>
+      <c r="T7" s="83"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="83"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="Y7" s="39" t="s">
+      <c r="Y7" s="29" t="s">
         <v>85</v>
       </c>
       <c r="Z7" s="5"/>
       <c r="AB7" s="4"/>
-      <c r="AC7" s="62" t="s">
+      <c r="AC7" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="AD7" s="57" t="s">
+      <c r="AD7" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="AE7" s="71"/>
-      <c r="AF7" s="71"/>
-      <c r="AG7" s="71"/>
-      <c r="AH7" s="58" t="s">
+      <c r="AE7" s="80"/>
+      <c r="AF7" s="80"/>
+      <c r="AG7" s="80"/>
+      <c r="AH7" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="AI7" s="59" t="s">
+      <c r="AI7" s="49" t="s">
         <v>97</v>
       </c>
       <c r="AJ7" s="5"/>
     </row>
     <row r="8" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="4"/>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="32" t="s">
         <v>55</v>
       </c>
       <c r="E8" s="73"/>
       <c r="F8" s="73"/>
       <c r="G8" s="73"/>
       <c r="H8" s="73"/>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="J8" s="29" t="s">
         <v>66</v>
       </c>
       <c r="K8" s="5"/>
@@ -2315,44 +2406,44 @@
     </row>
     <row r="9" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="4"/>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="33" t="s">
         <v>56</v>
       </c>
       <c r="E9" s="74"/>
       <c r="F9" s="74"/>
       <c r="G9" s="74"/>
       <c r="H9" s="74"/>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="29" t="s">
         <v>65</v>
       </c>
       <c r="K9" s="5"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="50" t="s">
+      <c r="N9" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="44" t="s">
+      <c r="O9" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P9" s="66" t="s">
+      <c r="P9" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="Q9" s="66"/>
-      <c r="R9" s="66"/>
-      <c r="S9" s="66"/>
-      <c r="T9" s="66"/>
-      <c r="U9" s="66"/>
-      <c r="V9" s="66"/>
-      <c r="W9" s="66"/>
-      <c r="X9" s="45" t="s">
+      <c r="Q9" s="81"/>
+      <c r="R9" s="81"/>
+      <c r="S9" s="81"/>
+      <c r="T9" s="81"/>
+      <c r="U9" s="81"/>
+      <c r="V9" s="81"/>
+      <c r="W9" s="81"/>
+      <c r="X9" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="Y9" s="39" t="s">
+      <c r="Y9" s="29" t="s">
         <v>84</v>
       </c>
       <c r="Z9" s="5"/>
@@ -2363,26 +2454,26 @@
       <c r="B10" s="4"/>
       <c r="K10" s="5"/>
       <c r="M10" s="4"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
-      <c r="S10" s="67"/>
-      <c r="T10" s="67"/>
-      <c r="U10" s="67"/>
-      <c r="V10" s="67"/>
-      <c r="W10" s="67"/>
-      <c r="X10" s="47"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="82"/>
+      <c r="S10" s="82"/>
+      <c r="T10" s="82"/>
+      <c r="U10" s="82"/>
+      <c r="V10" s="82"/>
+      <c r="W10" s="82"/>
+      <c r="X10" s="37"/>
       <c r="Z10" s="5"/>
       <c r="AB10" s="4"/>
       <c r="AJ10" s="5"/>
     </row>
     <row r="11" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="4"/>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="30" t="s">
         <v>57</v>
       </c>
       <c r="E11" s="72" t="s">
@@ -2391,29 +2482,29 @@
       <c r="F11" s="72"/>
       <c r="G11" s="72"/>
       <c r="H11" s="72"/>
-      <c r="I11" s="34" t="s">
+      <c r="I11" s="24" t="s">
         <v>59</v>
       </c>
       <c r="K11" s="5"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="51" t="s">
+      <c r="N11" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="O11" s="48" t="s">
+      <c r="O11" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="68"/>
-      <c r="Q11" s="68"/>
-      <c r="R11" s="68"/>
-      <c r="S11" s="68"/>
-      <c r="T11" s="68"/>
-      <c r="U11" s="68"/>
-      <c r="V11" s="68"/>
-      <c r="W11" s="68"/>
-      <c r="X11" s="49" t="s">
+      <c r="P11" s="83"/>
+      <c r="Q11" s="83"/>
+      <c r="R11" s="83"/>
+      <c r="S11" s="83"/>
+      <c r="T11" s="83"/>
+      <c r="U11" s="83"/>
+      <c r="V11" s="83"/>
+      <c r="W11" s="83"/>
+      <c r="X11" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="Y11" s="39" t="s">
+      <c r="Y11" s="29" t="s">
         <v>82</v>
       </c>
       <c r="Z11" s="5"/>
@@ -2422,17 +2513,17 @@
     </row>
     <row r="12" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="4"/>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="31" t="s">
         <v>58</v>
       </c>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
       <c r="G12" s="73"/>
       <c r="H12" s="73"/>
-      <c r="I12" s="35" t="s">
+      <c r="I12" s="25" t="s">
         <v>60</v>
       </c>
       <c r="K12" s="5"/>
@@ -2451,26 +2542,26 @@
       <c r="I13" s="5"/>
       <c r="K13" s="5"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="50" t="s">
+      <c r="N13" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="44" t="s">
+      <c r="O13" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P13" s="66" t="s">
+      <c r="P13" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="66"/>
-      <c r="S13" s="66"/>
-      <c r="T13" s="66"/>
-      <c r="U13" s="66"/>
-      <c r="V13" s="66"/>
-      <c r="W13" s="66"/>
-      <c r="X13" s="45" t="s">
+      <c r="Q13" s="81"/>
+      <c r="R13" s="81"/>
+      <c r="S13" s="81"/>
+      <c r="T13" s="81"/>
+      <c r="U13" s="81"/>
+      <c r="V13" s="81"/>
+      <c r="W13" s="81"/>
+      <c r="X13" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="Y13" s="39" t="s">
+      <c r="Y13" s="29" t="s">
         <v>88</v>
       </c>
       <c r="Z13" s="5"/>
@@ -2479,76 +2570,76 @@
     </row>
     <row r="14" spans="2:42" x14ac:dyDescent="0.45">
       <c r="B14" s="4"/>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="32" t="s">
         <v>55</v>
       </c>
       <c r="E14" s="73"/>
       <c r="F14" s="73"/>
       <c r="G14" s="73"/>
       <c r="H14" s="73"/>
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="39" t="s">
+      <c r="J14" s="29" t="s">
         <v>69</v>
       </c>
       <c r="K14" s="5"/>
       <c r="M14" s="4"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="67"/>
-      <c r="Q14" s="67"/>
-      <c r="R14" s="67"/>
-      <c r="S14" s="67"/>
-      <c r="T14" s="67"/>
-      <c r="U14" s="67"/>
-      <c r="V14" s="67"/>
-      <c r="W14" s="67"/>
-      <c r="X14" s="47"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="82"/>
+      <c r="R14" s="82"/>
+      <c r="S14" s="82"/>
+      <c r="T14" s="82"/>
+      <c r="U14" s="82"/>
+      <c r="V14" s="82"/>
+      <c r="W14" s="82"/>
+      <c r="X14" s="37"/>
       <c r="Z14" s="5"/>
       <c r="AB14" s="4"/>
       <c r="AJ14" s="5"/>
     </row>
     <row r="15" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="4"/>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="33" t="s">
         <v>56</v>
       </c>
       <c r="E15" s="74"/>
       <c r="F15" s="74"/>
       <c r="G15" s="74"/>
       <c r="H15" s="74"/>
-      <c r="I15" s="37" t="s">
+      <c r="I15" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="29" t="s">
         <v>68</v>
       </c>
       <c r="K15" s="5"/>
       <c r="M15" s="4"/>
-      <c r="N15" s="51" t="s">
+      <c r="N15" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="O15" s="48" t="s">
+      <c r="O15" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P15" s="68"/>
-      <c r="Q15" s="68"/>
-      <c r="R15" s="68"/>
-      <c r="S15" s="68"/>
-      <c r="T15" s="68"/>
-      <c r="U15" s="68"/>
-      <c r="V15" s="68"/>
-      <c r="W15" s="68"/>
-      <c r="X15" s="49" t="s">
+      <c r="P15" s="83"/>
+      <c r="Q15" s="83"/>
+      <c r="R15" s="83"/>
+      <c r="S15" s="83"/>
+      <c r="T15" s="83"/>
+      <c r="U15" s="83"/>
+      <c r="V15" s="83"/>
+      <c r="W15" s="83"/>
+      <c r="X15" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="Y15" s="39" t="s">
+      <c r="Y15" s="29" t="s">
         <v>89</v>
       </c>
       <c r="Z15" s="5"/>
@@ -2572,10 +2663,10 @@
     </row>
     <row r="17" spans="2:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B17" s="4"/>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="30" t="s">
         <v>57</v>
       </c>
       <c r="E17" s="72" t="s">
@@ -2584,74 +2675,74 @@
       <c r="F17" s="72"/>
       <c r="G17" s="72"/>
       <c r="H17" s="72"/>
-      <c r="I17" s="34" t="s">
+      <c r="I17" s="24" t="s">
         <v>59</v>
       </c>
       <c r="K17" s="5"/>
       <c r="M17" s="4"/>
-      <c r="N17" s="50" t="s">
+      <c r="N17" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="O17" s="44" t="s">
+      <c r="O17" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P17" s="66" t="s">
+      <c r="P17" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="66"/>
-      <c r="S17" s="66"/>
-      <c r="T17" s="66"/>
-      <c r="U17" s="66"/>
-      <c r="V17" s="66"/>
-      <c r="W17" s="66"/>
-      <c r="X17" s="45" t="s">
+      <c r="Q17" s="81"/>
+      <c r="R17" s="81"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
+      <c r="U17" s="81"/>
+      <c r="V17" s="81"/>
+      <c r="W17" s="81"/>
+      <c r="X17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="Y17" s="39" t="s">
+      <c r="Y17" s="29" t="s">
         <v>90</v>
       </c>
       <c r="Z17" s="5"/>
     </row>
     <row r="18" spans="2:36" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B18" s="4"/>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="31" t="s">
         <v>58</v>
       </c>
       <c r="E18" s="73"/>
       <c r="F18" s="73"/>
       <c r="G18" s="73"/>
       <c r="H18" s="73"/>
-      <c r="I18" s="35" t="s">
+      <c r="I18" s="25" t="s">
         <v>60</v>
       </c>
       <c r="K18" s="5"/>
       <c r="M18" s="4"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="67"/>
-      <c r="Q18" s="67"/>
-      <c r="R18" s="67"/>
-      <c r="S18" s="67"/>
-      <c r="T18" s="67"/>
-      <c r="U18" s="67"/>
-      <c r="V18" s="67"/>
-      <c r="W18" s="67"/>
-      <c r="X18" s="47"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="82"/>
+      <c r="Q18" s="82"/>
+      <c r="R18" s="82"/>
+      <c r="S18" s="82"/>
+      <c r="T18" s="82"/>
+      <c r="U18" s="82"/>
+      <c r="V18" s="82"/>
+      <c r="W18" s="82"/>
+      <c r="X18" s="37"/>
       <c r="Z18" s="5"/>
-      <c r="AB18" s="63" t="s">
+      <c r="AB18" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="AC18" s="64"/>
-      <c r="AD18" s="64"/>
-      <c r="AE18" s="64"/>
-      <c r="AF18" s="64"/>
-      <c r="AG18" s="64"/>
-      <c r="AH18" s="64"/>
-      <c r="AI18" s="64"/>
-      <c r="AJ18" s="65"/>
+      <c r="AC18" s="76"/>
+      <c r="AD18" s="76"/>
+      <c r="AE18" s="76"/>
+      <c r="AF18" s="76"/>
+      <c r="AG18" s="76"/>
+      <c r="AH18" s="76"/>
+      <c r="AI18" s="76"/>
+      <c r="AJ18" s="77"/>
     </row>
     <row r="19" spans="2:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="4"/>
@@ -2663,24 +2754,24 @@
       <c r="I19" s="5"/>
       <c r="K19" s="5"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="51" t="s">
+      <c r="N19" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="O19" s="48" t="s">
+      <c r="O19" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P19" s="68"/>
-      <c r="Q19" s="68"/>
-      <c r="R19" s="68"/>
-      <c r="S19" s="68"/>
-      <c r="T19" s="68"/>
-      <c r="U19" s="68"/>
-      <c r="V19" s="68"/>
-      <c r="W19" s="68"/>
-      <c r="X19" s="49" t="s">
+      <c r="P19" s="83"/>
+      <c r="Q19" s="83"/>
+      <c r="R19" s="83"/>
+      <c r="S19" s="83"/>
+      <c r="T19" s="83"/>
+      <c r="U19" s="83"/>
+      <c r="V19" s="83"/>
+      <c r="W19" s="83"/>
+      <c r="X19" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="Y19" s="39" t="s">
+      <c r="Y19" s="29" t="s">
         <v>91</v>
       </c>
       <c r="Z19" s="5"/>
@@ -2696,71 +2787,71 @@
     </row>
     <row r="20" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B20" s="4"/>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="32" t="s">
         <v>55</v>
       </c>
       <c r="E20" s="73"/>
       <c r="F20" s="73"/>
       <c r="G20" s="73"/>
       <c r="H20" s="73"/>
-      <c r="I20" s="36" t="s">
+      <c r="I20" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="J20" s="39" t="s">
+      <c r="J20" s="29" t="s">
         <v>72</v>
       </c>
       <c r="K20" s="5"/>
       <c r="M20" s="4"/>
       <c r="Z20" s="5"/>
       <c r="AB20" s="4"/>
-      <c r="AC20" s="62" t="s">
+      <c r="AC20" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="AD20" s="53" t="s">
+      <c r="AD20" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="AE20" s="69" t="s">
+      <c r="AE20" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="AF20" s="69"/>
-      <c r="AG20" s="69"/>
+      <c r="AF20" s="78"/>
+      <c r="AG20" s="78"/>
       <c r="AH20" s="3"/>
       <c r="AJ20" s="5"/>
     </row>
     <row r="21" spans="2:36" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B21" s="4"/>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="33" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="74"/>
       <c r="F21" s="74"/>
       <c r="G21" s="74"/>
       <c r="H21" s="74"/>
-      <c r="I21" s="37" t="s">
+      <c r="I21" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="J21" s="39" t="s">
+      <c r="J21" s="29" t="s">
         <v>71</v>
       </c>
       <c r="K21" s="5"/>
       <c r="M21" s="4"/>
       <c r="Z21" s="5"/>
       <c r="AB21" s="4"/>
-      <c r="AC21" s="61"/>
-      <c r="AD21" s="55"/>
+      <c r="AC21" s="51"/>
+      <c r="AD21" s="45"/>
       <c r="AE21" s="79"/>
       <c r="AF21" s="79"/>
       <c r="AG21" s="79"/>
-      <c r="AH21" s="80" t="s">
+      <c r="AH21" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="AI21" s="59" t="s">
+      <c r="AI21" s="49" t="s">
         <v>102</v>
       </c>
       <c r="AJ21" s="5"/>
@@ -2771,24 +2862,24 @@
       <c r="M22" s="4"/>
       <c r="Z22" s="5"/>
       <c r="AB22" s="4"/>
-      <c r="AC22" s="62" t="s">
+      <c r="AC22" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="AD22" s="57" t="s">
+      <c r="AD22" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="AE22" s="71"/>
-      <c r="AF22" s="71"/>
-      <c r="AG22" s="71"/>
+      <c r="AE22" s="80"/>
+      <c r="AF22" s="80"/>
+      <c r="AG22" s="80"/>
       <c r="AH22" s="8"/>
       <c r="AJ22" s="5"/>
     </row>
     <row r="23" spans="2:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="4"/>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="30" t="s">
         <v>57</v>
       </c>
       <c r="E23" s="72" t="s">
@@ -2797,52 +2888,45 @@
       <c r="F23" s="72"/>
       <c r="G23" s="72"/>
       <c r="H23" s="72"/>
-      <c r="I23" s="34" t="s">
+      <c r="I23" s="24" t="s">
         <v>59</v>
       </c>
       <c r="K23" s="5"/>
       <c r="M23" s="4"/>
       <c r="Z23" s="5"/>
       <c r="AB23" s="4"/>
-      <c r="AC23" s="78"/>
-      <c r="AD23" s="78"/>
-      <c r="AE23" s="78"/>
-      <c r="AF23" s="78"/>
-      <c r="AG23" s="78"/>
-      <c r="AH23" s="78"/>
-      <c r="AI23" s="78"/>
       <c r="AJ23" s="5"/>
     </row>
     <row r="24" spans="2:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="4"/>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="41" t="s">
+      <c r="D24" s="31" t="s">
         <v>58</v>
       </c>
       <c r="E24" s="73"/>
       <c r="F24" s="73"/>
       <c r="G24" s="73"/>
       <c r="H24" s="73"/>
-      <c r="I24" s="35" t="s">
+      <c r="I24" s="25" t="s">
         <v>60</v>
       </c>
       <c r="K24" s="5"/>
       <c r="M24" s="4"/>
       <c r="Z24" s="5"/>
       <c r="AB24" s="4"/>
-      <c r="AC24" s="62" t="s">
+      <c r="AC24" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="AD24" s="53" t="s">
+      <c r="AD24" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="AE24" s="69" t="s">
+      <c r="AE24" s="78" t="s">
         <v>100</v>
       </c>
-      <c r="AF24" s="69"/>
-      <c r="AG24" s="69"/>
+      <c r="AF24" s="78"/>
+      <c r="AG24" s="78"/>
       <c r="AH24" s="3"/>
       <c r="AJ24" s="5"/>
     </row>
@@ -2858,82 +2942,75 @@
       <c r="M25" s="4"/>
       <c r="Z25" s="5"/>
       <c r="AB25" s="4"/>
-      <c r="AC25" s="61"/>
-      <c r="AD25" s="55"/>
+      <c r="AC25" s="51"/>
+      <c r="AD25" s="45"/>
       <c r="AE25" s="79"/>
       <c r="AF25" s="79"/>
       <c r="AG25" s="79"/>
-      <c r="AH25" s="80" t="s">
+      <c r="AH25" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="AI25" s="59" t="s">
+      <c r="AI25" s="49" t="s">
         <v>1</v>
       </c>
       <c r="AJ25" s="5"/>
     </row>
     <row r="26" spans="2:36" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B26" s="4"/>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="32" t="s">
         <v>55</v>
       </c>
       <c r="E26" s="73"/>
       <c r="F26" s="73"/>
       <c r="G26" s="73"/>
       <c r="H26" s="73"/>
-      <c r="I26" s="36" t="s">
+      <c r="I26" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="J26" s="39" t="s">
+      <c r="J26" s="29" t="s">
         <v>75</v>
       </c>
       <c r="K26" s="5"/>
       <c r="M26" s="4"/>
       <c r="Z26" s="5"/>
       <c r="AB26" s="4"/>
-      <c r="AC26" s="62" t="s">
+      <c r="AC26" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="AD26" s="57" t="s">
+      <c r="AD26" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="AE26" s="71"/>
-      <c r="AF26" s="71"/>
-      <c r="AG26" s="71"/>
+      <c r="AE26" s="80"/>
+      <c r="AF26" s="80"/>
+      <c r="AG26" s="80"/>
       <c r="AH26" s="8"/>
       <c r="AJ26" s="5"/>
     </row>
     <row r="27" spans="2:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="4"/>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="33" t="s">
         <v>56</v>
       </c>
       <c r="E27" s="74"/>
       <c r="F27" s="74"/>
       <c r="G27" s="74"/>
       <c r="H27" s="74"/>
-      <c r="I27" s="37" t="s">
+      <c r="I27" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="J27" s="39" t="s">
+      <c r="J27" s="29" t="s">
         <v>74</v>
       </c>
       <c r="K27" s="5"/>
       <c r="M27" s="4"/>
       <c r="Z27" s="5"/>
       <c r="AB27" s="4"/>
-      <c r="AC27" s="78"/>
-      <c r="AD27" s="78"/>
-      <c r="AE27" s="78"/>
-      <c r="AF27" s="78"/>
-      <c r="AG27" s="78"/>
-      <c r="AH27" s="78"/>
-      <c r="AI27" s="78"/>
       <c r="AJ27" s="5"/>
     </row>
     <row r="28" spans="2:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -2971,39 +3048,6 @@
       <c r="AI28" s="7"/>
       <c r="AJ28" s="8"/>
     </row>
-    <row r="29" spans="2:36" x14ac:dyDescent="0.45">
-      <c r="AB29" s="78"/>
-      <c r="AC29" s="78"/>
-      <c r="AD29" s="78"/>
-      <c r="AE29" s="78"/>
-      <c r="AF29" s="78"/>
-      <c r="AG29" s="78"/>
-      <c r="AH29" s="78"/>
-      <c r="AI29" s="78"/>
-      <c r="AJ29" s="78"/>
-    </row>
-    <row r="30" spans="2:36" x14ac:dyDescent="0.45">
-      <c r="AB30" s="78"/>
-      <c r="AC30" s="78"/>
-      <c r="AD30" s="78"/>
-      <c r="AE30" s="78"/>
-      <c r="AF30" s="78"/>
-      <c r="AG30" s="78"/>
-      <c r="AH30" s="78"/>
-      <c r="AI30" s="78"/>
-      <c r="AJ30" s="78"/>
-    </row>
-    <row r="31" spans="2:36" x14ac:dyDescent="0.45">
-      <c r="AB31" s="78"/>
-      <c r="AC31" s="78"/>
-      <c r="AD31" s="78"/>
-      <c r="AE31" s="78"/>
-      <c r="AF31" s="78"/>
-      <c r="AG31" s="78"/>
-      <c r="AH31" s="78"/>
-      <c r="AI31" s="78"/>
-      <c r="AJ31" s="78"/>
-    </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="E23:H27"/>

</xml_diff>

<commit_message>
Added ultrasonic sensor to main loop and confirmed telem
</commit_message>
<xml_diff>
--- a/electrical_hardware/APWCR_Electrical_Pin_Connections.xlsx
+++ b/electrical_hardware/APWCR_Electrical_Pin_Connections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\UT_Files\Senior_Design_Repos\APWCR_Software\electrical_hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8E3E6B-DC21-4ACA-80B5-31AF7D02D4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD728E74-41B6-4080-9C88-A077446C11CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Layout" sheetId="1" r:id="rId1"/>
@@ -319,12 +319,6 @@
     <t>Echo</t>
   </si>
   <si>
-    <t>D25</t>
-  </si>
-  <si>
-    <t>D24</t>
-  </si>
-  <si>
     <t>MG996R Servo - Lid</t>
   </si>
   <si>
@@ -365,6 +359,12 @@
   </si>
   <si>
     <t>HC-SR04 VCC</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
   </si>
 </sst>
 </file>
@@ -1053,6 +1053,15 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1087,15 +1096,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1380,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1393,26 +1393,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="86"/>
-      <c r="S2" s="86"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B3" s="9"/>
@@ -1439,10 +1439,10 @@
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="68" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F4" s="69" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
@@ -1454,7 +1454,7 @@
       <c r="N4" s="54"/>
       <c r="O4" s="54"/>
       <c r="P4" s="69" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
@@ -1512,20 +1512,20 @@
       <c r="D6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="84" t="s">
+      <c r="E6" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="84"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
       <c r="Q6" s="19" t="s">
         <v>25</v>
       </c>
@@ -1540,18 +1540,18 @@
       <c r="D7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="84"/>
-      <c r="M7" s="84"/>
-      <c r="N7" s="84"/>
-      <c r="O7" s="84"/>
-      <c r="P7" s="84"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="72"/>
       <c r="Q7" s="19" t="s">
         <v>26</v>
       </c>
@@ -1607,10 +1607,10 @@
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="70" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F9" s="71" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G9" s="55" t="s">
         <v>31</v>
@@ -1734,20 +1734,20 @@
       <c r="D13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="85" t="s">
+      <c r="E13" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="85"/>
-      <c r="K13" s="85"/>
-      <c r="L13" s="85"/>
-      <c r="M13" s="85"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="85"/>
-      <c r="P13" s="85"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="73"/>
       <c r="Q13" s="20" t="s">
         <v>25</v>
       </c>
@@ -1762,18 +1762,18 @@
       <c r="D14" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
-      <c r="K14" s="85"/>
-      <c r="L14" s="85"/>
-      <c r="M14" s="85"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="73"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73"/>
+      <c r="L14" s="73"/>
+      <c r="M14" s="73"/>
+      <c r="N14" s="73"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="73"/>
       <c r="Q14" s="20" t="s">
         <v>26</v>
       </c>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="G16" s="62"/>
       <c r="H16" s="61" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I16" s="62"/>
       <c r="J16" s="62"/>
@@ -1886,17 +1886,17 @@
       </c>
       <c r="G18" s="67"/>
       <c r="H18" s="66" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I18" s="67"/>
       <c r="J18" s="67"/>
       <c r="K18" s="67"/>
       <c r="L18" s="67"/>
       <c r="M18" s="65" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N18" s="66" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O18" s="65" t="s">
         <v>47</v>
@@ -1960,20 +1960,20 @@
       <c r="D20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="85" t="s">
+      <c r="E20" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="85"/>
-      <c r="I20" s="85"/>
-      <c r="J20" s="85"/>
-      <c r="K20" s="85"/>
-      <c r="L20" s="85"/>
-      <c r="M20" s="85"/>
-      <c r="N20" s="85"/>
-      <c r="O20" s="85"/>
-      <c r="P20" s="85"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="73"/>
       <c r="Q20" s="20" t="s">
         <v>25</v>
       </c>
@@ -1988,18 +1988,18 @@
       <c r="D21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="85"/>
-      <c r="F21" s="85"/>
-      <c r="G21" s="85"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="85"/>
-      <c r="J21" s="85"/>
-      <c r="K21" s="85"/>
-      <c r="L21" s="85"/>
-      <c r="M21" s="85"/>
-      <c r="N21" s="85"/>
-      <c r="O21" s="85"/>
-      <c r="P21" s="85"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="73"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="73"/>
       <c r="Q21" s="20" t="s">
         <v>26</v>
       </c>
@@ -2135,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4C9B7A-925E-4ACB-8F3D-3CC4DA199EDA}">
   <dimension ref="B2:AP28"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AI31" sqref="AI31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2150,45 +2150,45 @@
   <sheetData>
     <row r="2" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="2:42" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="77"/>
-      <c r="M3" s="75" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="80"/>
+      <c r="M3" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="76"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="76"/>
-      <c r="X3" s="76"/>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="77"/>
-      <c r="AB3" s="75" t="s">
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="79"/>
+      <c r="S3" s="79"/>
+      <c r="T3" s="79"/>
+      <c r="U3" s="79"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
+      <c r="X3" s="79"/>
+      <c r="Y3" s="79"/>
+      <c r="Z3" s="80"/>
+      <c r="AB3" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="AC3" s="76"/>
-      <c r="AD3" s="76"/>
-      <c r="AE3" s="76"/>
-      <c r="AF3" s="76"/>
-      <c r="AG3" s="76"/>
-      <c r="AH3" s="76"/>
-      <c r="AI3" s="76"/>
-      <c r="AJ3" s="77"/>
+      <c r="AC3" s="79"/>
+      <c r="AD3" s="79"/>
+      <c r="AE3" s="79"/>
+      <c r="AF3" s="79"/>
+      <c r="AG3" s="79"/>
+      <c r="AH3" s="79"/>
+      <c r="AI3" s="79"/>
+      <c r="AJ3" s="80"/>
       <c r="AK3" s="42"/>
       <c r="AL3" s="42"/>
       <c r="AM3" s="42"/>
@@ -2239,12 +2239,12 @@
       <c r="D5" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
       <c r="I5" s="24" t="s">
         <v>59</v>
       </c>
@@ -2256,16 +2256,16 @@
       <c r="O5" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="81" t="s">
+      <c r="P5" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="84"/>
+      <c r="S5" s="84"/>
+      <c r="T5" s="84"/>
+      <c r="U5" s="84"/>
+      <c r="V5" s="84"/>
+      <c r="W5" s="84"/>
       <c r="X5" s="35" t="s">
         <v>78</v>
       </c>
@@ -2280,16 +2280,16 @@
       <c r="AD5" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="AE5" s="78" t="s">
+      <c r="AE5" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="AF5" s="78"/>
-      <c r="AG5" s="78"/>
+      <c r="AF5" s="81"/>
+      <c r="AG5" s="81"/>
       <c r="AH5" s="44" t="s">
         <v>95</v>
       </c>
       <c r="AI5" s="49" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="AJ5" s="5"/>
     </row>
@@ -2301,32 +2301,32 @@
       <c r="D6" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
       <c r="I6" s="25" t="s">
         <v>60</v>
       </c>
       <c r="K6" s="5"/>
       <c r="M6" s="4"/>
       <c r="O6" s="36"/>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
-      <c r="S6" s="82"/>
-      <c r="T6" s="82"/>
-      <c r="U6" s="82"/>
-      <c r="V6" s="82"/>
-      <c r="W6" s="82"/>
+      <c r="P6" s="85"/>
+      <c r="Q6" s="85"/>
+      <c r="R6" s="85"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="85"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="85"/>
+      <c r="W6" s="85"/>
       <c r="X6" s="37"/>
       <c r="Z6" s="5"/>
       <c r="AB6" s="4"/>
       <c r="AC6" s="51"/>
       <c r="AD6" s="45"/>
-      <c r="AE6" s="79"/>
-      <c r="AF6" s="79"/>
-      <c r="AG6" s="79"/>
+      <c r="AE6" s="82"/>
+      <c r="AF6" s="82"/>
+      <c r="AG6" s="82"/>
       <c r="AH6" s="46"/>
       <c r="AI6" s="50"/>
       <c r="AJ6" s="5"/>
@@ -2334,10 +2334,10 @@
     <row r="7" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
       <c r="I7" s="5"/>
       <c r="K7" s="5"/>
       <c r="M7" s="4"/>
@@ -2347,14 +2347,14 @@
       <c r="O7" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P7" s="83"/>
-      <c r="Q7" s="83"/>
-      <c r="R7" s="83"/>
-      <c r="S7" s="83"/>
-      <c r="T7" s="83"/>
-      <c r="U7" s="83"/>
-      <c r="V7" s="83"/>
-      <c r="W7" s="83"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="86"/>
+      <c r="S7" s="86"/>
+      <c r="T7" s="86"/>
+      <c r="U7" s="86"/>
+      <c r="V7" s="86"/>
+      <c r="W7" s="86"/>
       <c r="X7" s="39" t="s">
         <v>79</v>
       </c>
@@ -2369,14 +2369,14 @@
       <c r="AD7" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="AE7" s="80"/>
-      <c r="AF7" s="80"/>
-      <c r="AG7" s="80"/>
+      <c r="AE7" s="83"/>
+      <c r="AF7" s="83"/>
+      <c r="AG7" s="83"/>
       <c r="AH7" s="48" t="s">
         <v>96</v>
       </c>
       <c r="AI7" s="49" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="AJ7" s="5"/>
     </row>
@@ -2388,10 +2388,10 @@
       <c r="D8" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
       <c r="I8" s="26" t="s">
         <v>61</v>
       </c>
@@ -2412,10 +2412,10 @@
       <c r="D9" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
       <c r="I9" s="27" t="s">
         <v>62</v>
       </c>
@@ -2430,16 +2430,16 @@
       <c r="O9" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P9" s="81" t="s">
+      <c r="P9" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="81"/>
-      <c r="S9" s="81"/>
-      <c r="T9" s="81"/>
-      <c r="U9" s="81"/>
-      <c r="V9" s="81"/>
-      <c r="W9" s="81"/>
+      <c r="Q9" s="84"/>
+      <c r="R9" s="84"/>
+      <c r="S9" s="84"/>
+      <c r="T9" s="84"/>
+      <c r="U9" s="84"/>
+      <c r="V9" s="84"/>
+      <c r="W9" s="84"/>
       <c r="X9" s="35" t="s">
         <v>78</v>
       </c>
@@ -2455,14 +2455,14 @@
       <c r="K10" s="5"/>
       <c r="M10" s="4"/>
       <c r="O10" s="36"/>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="82"/>
-      <c r="R10" s="82"/>
-      <c r="S10" s="82"/>
-      <c r="T10" s="82"/>
-      <c r="U10" s="82"/>
-      <c r="V10" s="82"/>
-      <c r="W10" s="82"/>
+      <c r="P10" s="85"/>
+      <c r="Q10" s="85"/>
+      <c r="R10" s="85"/>
+      <c r="S10" s="85"/>
+      <c r="T10" s="85"/>
+      <c r="U10" s="85"/>
+      <c r="V10" s="85"/>
+      <c r="W10" s="85"/>
       <c r="X10" s="37"/>
       <c r="Z10" s="5"/>
       <c r="AB10" s="4"/>
@@ -2476,12 +2476,12 @@
       <c r="D11" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
       <c r="I11" s="24" t="s">
         <v>59</v>
       </c>
@@ -2493,14 +2493,14 @@
       <c r="O11" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="83"/>
-      <c r="Q11" s="83"/>
-      <c r="R11" s="83"/>
-      <c r="S11" s="83"/>
-      <c r="T11" s="83"/>
-      <c r="U11" s="83"/>
-      <c r="V11" s="83"/>
-      <c r="W11" s="83"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
+      <c r="T11" s="86"/>
+      <c r="U11" s="86"/>
+      <c r="V11" s="86"/>
+      <c r="W11" s="86"/>
       <c r="X11" s="39" t="s">
         <v>79</v>
       </c>
@@ -2519,10 +2519,10 @@
       <c r="D12" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
       <c r="I12" s="25" t="s">
         <v>60</v>
       </c>
@@ -2535,10 +2535,10 @@
     <row r="13" spans="2:42" x14ac:dyDescent="0.45">
       <c r="B13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
       <c r="I13" s="5"/>
       <c r="K13" s="5"/>
       <c r="M13" s="4"/>
@@ -2548,16 +2548,16 @@
       <c r="O13" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P13" s="81" t="s">
+      <c r="P13" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="Q13" s="81"/>
-      <c r="R13" s="81"/>
-      <c r="S13" s="81"/>
-      <c r="T13" s="81"/>
-      <c r="U13" s="81"/>
-      <c r="V13" s="81"/>
-      <c r="W13" s="81"/>
+      <c r="Q13" s="84"/>
+      <c r="R13" s="84"/>
+      <c r="S13" s="84"/>
+      <c r="T13" s="84"/>
+      <c r="U13" s="84"/>
+      <c r="V13" s="84"/>
+      <c r="W13" s="84"/>
       <c r="X13" s="35" t="s">
         <v>78</v>
       </c>
@@ -2576,10 +2576,10 @@
       <c r="D14" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
       <c r="I14" s="26" t="s">
         <v>61</v>
       </c>
@@ -2589,14 +2589,14 @@
       <c r="K14" s="5"/>
       <c r="M14" s="4"/>
       <c r="O14" s="36"/>
-      <c r="P14" s="82"/>
-      <c r="Q14" s="82"/>
-      <c r="R14" s="82"/>
-      <c r="S14" s="82"/>
-      <c r="T14" s="82"/>
-      <c r="U14" s="82"/>
-      <c r="V14" s="82"/>
-      <c r="W14" s="82"/>
+      <c r="P14" s="85"/>
+      <c r="Q14" s="85"/>
+      <c r="R14" s="85"/>
+      <c r="S14" s="85"/>
+      <c r="T14" s="85"/>
+      <c r="U14" s="85"/>
+      <c r="V14" s="85"/>
+      <c r="W14" s="85"/>
       <c r="X14" s="37"/>
       <c r="Z14" s="5"/>
       <c r="AB14" s="4"/>
@@ -2610,10 +2610,10 @@
       <c r="D15" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="77"/>
       <c r="I15" s="27" t="s">
         <v>62</v>
       </c>
@@ -2628,14 +2628,14 @@
       <c r="O15" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="83"/>
-      <c r="R15" s="83"/>
-      <c r="S15" s="83"/>
-      <c r="T15" s="83"/>
-      <c r="U15" s="83"/>
-      <c r="V15" s="83"/>
-      <c r="W15" s="83"/>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="86"/>
+      <c r="R15" s="86"/>
+      <c r="S15" s="86"/>
+      <c r="T15" s="86"/>
+      <c r="U15" s="86"/>
+      <c r="V15" s="86"/>
+      <c r="W15" s="86"/>
       <c r="X15" s="39" t="s">
         <v>79</v>
       </c>
@@ -2669,12 +2669,12 @@
       <c r="D17" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="72" t="s">
+      <c r="E17" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
       <c r="I17" s="24" t="s">
         <v>59</v>
       </c>
@@ -2686,16 +2686,16 @@
       <c r="O17" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P17" s="81" t="s">
+      <c r="P17" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="81"/>
-      <c r="S17" s="81"/>
-      <c r="T17" s="81"/>
-      <c r="U17" s="81"/>
-      <c r="V17" s="81"/>
-      <c r="W17" s="81"/>
+      <c r="Q17" s="84"/>
+      <c r="R17" s="84"/>
+      <c r="S17" s="84"/>
+      <c r="T17" s="84"/>
+      <c r="U17" s="84"/>
+      <c r="V17" s="84"/>
+      <c r="W17" s="84"/>
       <c r="X17" s="35" t="s">
         <v>78</v>
       </c>
@@ -2712,45 +2712,45 @@
       <c r="D18" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
       <c r="I18" s="25" t="s">
         <v>60</v>
       </c>
       <c r="K18" s="5"/>
       <c r="M18" s="4"/>
       <c r="O18" s="36"/>
-      <c r="P18" s="82"/>
-      <c r="Q18" s="82"/>
-      <c r="R18" s="82"/>
-      <c r="S18" s="82"/>
-      <c r="T18" s="82"/>
-      <c r="U18" s="82"/>
-      <c r="V18" s="82"/>
-      <c r="W18" s="82"/>
+      <c r="P18" s="85"/>
+      <c r="Q18" s="85"/>
+      <c r="R18" s="85"/>
+      <c r="S18" s="85"/>
+      <c r="T18" s="85"/>
+      <c r="U18" s="85"/>
+      <c r="V18" s="85"/>
+      <c r="W18" s="85"/>
       <c r="X18" s="37"/>
       <c r="Z18" s="5"/>
-      <c r="AB18" s="75" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC18" s="76"/>
-      <c r="AD18" s="76"/>
-      <c r="AE18" s="76"/>
-      <c r="AF18" s="76"/>
-      <c r="AG18" s="76"/>
-      <c r="AH18" s="76"/>
-      <c r="AI18" s="76"/>
-      <c r="AJ18" s="77"/>
+      <c r="AB18" s="78" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC18" s="79"/>
+      <c r="AD18" s="79"/>
+      <c r="AE18" s="79"/>
+      <c r="AF18" s="79"/>
+      <c r="AG18" s="79"/>
+      <c r="AH18" s="79"/>
+      <c r="AI18" s="79"/>
+      <c r="AJ18" s="80"/>
     </row>
     <row r="19" spans="2:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
       <c r="I19" s="5"/>
       <c r="K19" s="5"/>
       <c r="M19" s="4"/>
@@ -2760,14 +2760,14 @@
       <c r="O19" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P19" s="83"/>
-      <c r="Q19" s="83"/>
-      <c r="R19" s="83"/>
-      <c r="S19" s="83"/>
-      <c r="T19" s="83"/>
-      <c r="U19" s="83"/>
-      <c r="V19" s="83"/>
-      <c r="W19" s="83"/>
+      <c r="P19" s="86"/>
+      <c r="Q19" s="86"/>
+      <c r="R19" s="86"/>
+      <c r="S19" s="86"/>
+      <c r="T19" s="86"/>
+      <c r="U19" s="86"/>
+      <c r="V19" s="86"/>
+      <c r="W19" s="86"/>
       <c r="X19" s="39" t="s">
         <v>79</v>
       </c>
@@ -2793,10 +2793,10 @@
       <c r="D20" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
       <c r="I20" s="26" t="s">
         <v>61</v>
       </c>
@@ -2813,11 +2813,11 @@
       <c r="AD20" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="AE20" s="78" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF20" s="78"/>
-      <c r="AG20" s="78"/>
+      <c r="AE20" s="81" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF20" s="81"/>
+      <c r="AG20" s="81"/>
       <c r="AH20" s="3"/>
       <c r="AJ20" s="5"/>
     </row>
@@ -2829,10 +2829,10 @@
       <c r="D21" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
       <c r="I21" s="27" t="s">
         <v>62</v>
       </c>
@@ -2845,14 +2845,14 @@
       <c r="AB21" s="4"/>
       <c r="AC21" s="51"/>
       <c r="AD21" s="45"/>
-      <c r="AE21" s="79"/>
-      <c r="AF21" s="79"/>
-      <c r="AG21" s="79"/>
+      <c r="AE21" s="82"/>
+      <c r="AF21" s="82"/>
+      <c r="AG21" s="82"/>
       <c r="AH21" s="53" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AI21" s="49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AJ21" s="5"/>
     </row>
@@ -2868,9 +2868,9 @@
       <c r="AD22" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="AE22" s="80"/>
-      <c r="AF22" s="80"/>
-      <c r="AG22" s="80"/>
+      <c r="AE22" s="83"/>
+      <c r="AF22" s="83"/>
+      <c r="AG22" s="83"/>
       <c r="AH22" s="8"/>
       <c r="AJ22" s="5"/>
     </row>
@@ -2882,12 +2882,12 @@
       <c r="D23" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="72" t="s">
+      <c r="E23" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
       <c r="I23" s="24" t="s">
         <v>59</v>
       </c>
@@ -2905,10 +2905,10 @@
       <c r="D24" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
       <c r="I24" s="25" t="s">
         <v>60</v>
       </c>
@@ -2922,21 +2922,21 @@
       <c r="AD24" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="AE24" s="78" t="s">
-        <v>100</v>
-      </c>
-      <c r="AF24" s="78"/>
-      <c r="AG24" s="78"/>
+      <c r="AE24" s="81" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF24" s="81"/>
+      <c r="AG24" s="81"/>
       <c r="AH24" s="3"/>
       <c r="AJ24" s="5"/>
     </row>
     <row r="25" spans="2:36" ht="19.5" x14ac:dyDescent="0.6">
       <c r="B25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="76"/>
       <c r="I25" s="5"/>
       <c r="K25" s="5"/>
       <c r="M25" s="4"/>
@@ -2944,11 +2944,11 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="51"/>
       <c r="AD25" s="45"/>
-      <c r="AE25" s="79"/>
-      <c r="AF25" s="79"/>
-      <c r="AG25" s="79"/>
+      <c r="AE25" s="82"/>
+      <c r="AF25" s="82"/>
+      <c r="AG25" s="82"/>
       <c r="AH25" s="53" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AI25" s="49" t="s">
         <v>1</v>
@@ -2963,10 +2963,10 @@
       <c r="D26" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
       <c r="I26" s="26" t="s">
         <v>61</v>
       </c>
@@ -2983,9 +2983,9 @@
       <c r="AD26" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="AE26" s="80"/>
-      <c r="AF26" s="80"/>
-      <c r="AG26" s="80"/>
+      <c r="AE26" s="83"/>
+      <c r="AF26" s="83"/>
+      <c r="AG26" s="83"/>
       <c r="AH26" s="8"/>
       <c r="AJ26" s="5"/>
     </row>
@@ -2997,10 +2997,10 @@
       <c r="D27" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="77"/>
       <c r="I27" s="27" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Added servo logic to python and arduino
</commit_message>
<xml_diff>
--- a/electrical_hardware/APWCR_Electrical_Pin_Connections.xlsx
+++ b/electrical_hardware/APWCR_Electrical_Pin_Connections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\UT_Files\Senior_Design_Repos\APWCR_Software\electrical_hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD728E74-41B6-4080-9C88-A077446C11CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC50C2D5-55A5-427D-A053-BD29FB099B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Layout" sheetId="1" r:id="rId1"/>
@@ -916,7 +916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1002,15 +1002,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1053,6 +1044,42 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1060,42 +1087,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1380,39 +1371,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="6.1328125" customWidth="1"/>
     <col min="4" max="4" width="3.59765625" customWidth="1"/>
-    <col min="5" max="16" width="12.53125" customWidth="1"/>
+    <col min="5" max="16" width="13.19921875" customWidth="1"/>
     <col min="17" max="17" width="3.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="74"/>
-      <c r="S2" s="74"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B3" s="9"/>
@@ -1438,10 +1429,10 @@
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="F4" s="69" t="s">
+      <c r="F4" s="66" t="s">
         <v>103</v>
       </c>
       <c r="G4" s="54"/>
@@ -1453,7 +1444,7 @@
       <c r="M4" s="54"/>
       <c r="N4" s="54"/>
       <c r="O4" s="54"/>
-      <c r="P4" s="69" t="s">
+      <c r="P4" s="66" t="s">
         <v>108</v>
       </c>
       <c r="Q4" s="13"/>
@@ -1464,40 +1455,40 @@
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="58" t="s">
+      <c r="G5" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="58" t="s">
+      <c r="H5" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="58" t="s">
+      <c r="I5" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="58" t="s">
+      <c r="K5" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="58" t="s">
+      <c r="L5" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="58" t="s">
+      <c r="M5" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="58" t="s">
+      <c r="N5" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="58" t="s">
+      <c r="O5" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="58" t="s">
+      <c r="P5" s="55" t="s">
         <v>24</v>
       </c>
       <c r="Q5" s="11"/>
@@ -1512,20 +1503,20 @@
       <c r="D6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="72" t="s">
+      <c r="E6" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="72"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="81"/>
       <c r="Q6" s="19" t="s">
         <v>25</v>
       </c>
@@ -1540,18 +1531,18 @@
       <c r="D7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="72"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
       <c r="Q7" s="19" t="s">
         <v>26</v>
       </c>
@@ -1562,82 +1553,82 @@
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="15"/>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="59" t="s">
+      <c r="K8" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="59" t="s">
+      <c r="L8" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="59" t="s">
+      <c r="M8" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="59" t="s">
+      <c r="N8" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="59" t="s">
+      <c r="O8" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="59" t="s">
+      <c r="P8" s="56" t="s">
         <v>12</v>
       </c>
       <c r="Q8" s="17"/>
       <c r="R8" s="13"/>
       <c r="S8" s="14"/>
     </row>
-    <row r="9" spans="2:19" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:19" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="70" t="s">
+      <c r="E9" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="71" t="s">
+      <c r="F9" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="55" t="s">
+      <c r="G9" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H9" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="55" t="s">
+      <c r="I9" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="55" t="s">
+      <c r="K9" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="56" t="s">
+      <c r="L9" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="M9" s="55" t="s">
+      <c r="M9" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="56" t="s">
+      <c r="N9" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="O9" s="57"/>
-      <c r="P9" s="57"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="59"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
       <c r="S9" s="14"/>
@@ -1686,40 +1677,40 @@
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="63" t="s">
+      <c r="E12" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="63" t="s">
+      <c r="F12" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="63" t="s">
+      <c r="G12" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="63" t="s">
+      <c r="H12" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="63" t="s">
+      <c r="I12" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="63" t="s">
+      <c r="J12" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="63" t="s">
+      <c r="K12" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="63" t="s">
+      <c r="L12" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="63" t="s">
+      <c r="M12" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="63" t="s">
+      <c r="N12" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="O12" s="63" t="s">
+      <c r="O12" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="P12" s="63" t="s">
+      <c r="P12" s="60" t="s">
         <v>24</v>
       </c>
       <c r="Q12" s="11"/>
@@ -1734,20 +1725,20 @@
       <c r="D13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="73" t="s">
+      <c r="E13" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="73"/>
-      <c r="O13" s="73"/>
-      <c r="P13" s="73"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="82"/>
       <c r="Q13" s="20" t="s">
         <v>25</v>
       </c>
@@ -1762,18 +1753,18 @@
       <c r="D14" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
-      <c r="O14" s="73"/>
-      <c r="P14" s="73"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="82"/>
       <c r="Q14" s="20" t="s">
         <v>26</v>
       </c>
@@ -1784,40 +1775,40 @@
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="64" t="s">
+      <c r="E15" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="64" t="s">
+      <c r="F15" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="64" t="s">
+      <c r="G15" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="64" t="s">
+      <c r="H15" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="64" t="s">
+      <c r="I15" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="64" t="s">
+      <c r="J15" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="64" t="s">
+      <c r="K15" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="L15" s="64" t="s">
+      <c r="L15" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="64" t="s">
+      <c r="M15" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="N15" s="64" t="s">
+      <c r="N15" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="O15" s="64" t="s">
+      <c r="O15" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="P15" s="64" t="s">
+      <c r="P15" s="61" t="s">
         <v>12</v>
       </c>
       <c r="Q15" s="17"/>
@@ -1828,26 +1819,26 @@
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="60" t="s">
+      <c r="E16" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="61" t="s">
+      <c r="F16" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="62"/>
-      <c r="H16" s="61" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="62"/>
-      <c r="N16" s="62"/>
-      <c r="O16" s="60" t="s">
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="P16" s="61" t="s">
+      <c r="P16" s="58" t="s">
         <v>42</v>
       </c>
       <c r="Q16" s="13"/>
@@ -1878,30 +1869,30 @@
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="65" t="s">
+      <c r="E18" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="66" t="s">
+      <c r="F18" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="67"/>
-      <c r="H18" s="66" t="s">
+      <c r="G18" s="64"/>
+      <c r="H18" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="65" t="s">
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="N18" s="66" t="s">
+      <c r="N18" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="O18" s="65" t="s">
+      <c r="O18" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="P18" s="66" t="s">
+      <c r="P18" s="63" t="s">
         <v>48</v>
       </c>
       <c r="Q18" s="13"/>
@@ -1912,40 +1903,40 @@
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="63" t="s">
+      <c r="E19" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="63" t="s">
+      <c r="F19" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="63" t="s">
+      <c r="G19" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="63" t="s">
+      <c r="H19" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="63" t="s">
+      <c r="I19" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="63" t="s">
+      <c r="J19" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="63" t="s">
+      <c r="K19" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="63" t="s">
+      <c r="L19" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="63" t="s">
+      <c r="M19" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="N19" s="63" t="s">
+      <c r="N19" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="63" t="s">
+      <c r="O19" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="P19" s="63" t="s">
+      <c r="P19" s="60" t="s">
         <v>24</v>
       </c>
       <c r="Q19" s="11"/>
@@ -1960,20 +1951,20 @@
       <c r="D20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="73" t="s">
+      <c r="E20" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="73"/>
-      <c r="N20" s="73"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="73"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="82"/>
+      <c r="O20" s="82"/>
+      <c r="P20" s="82"/>
       <c r="Q20" s="20" t="s">
         <v>25</v>
       </c>
@@ -1988,18 +1979,18 @@
       <c r="D21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="73"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="73"/>
-      <c r="N21" s="73"/>
-      <c r="O21" s="73"/>
-      <c r="P21" s="73"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="82"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="82"/>
+      <c r="N21" s="82"/>
+      <c r="O21" s="82"/>
+      <c r="P21" s="82"/>
       <c r="Q21" s="20" t="s">
         <v>26</v>
       </c>
@@ -2010,40 +2001,40 @@
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="64" t="s">
+      <c r="E22" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="64" t="s">
+      <c r="G22" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="64" t="s">
+      <c r="H22" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="64" t="s">
+      <c r="I22" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="64" t="s">
+      <c r="J22" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="K22" s="64" t="s">
+      <c r="K22" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="64" t="s">
+      <c r="L22" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="64" t="s">
+      <c r="M22" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="N22" s="64" t="s">
+      <c r="N22" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="O22" s="64" t="s">
+      <c r="O22" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="P22" s="64" t="s">
+      <c r="P22" s="61" t="s">
         <v>12</v>
       </c>
       <c r="Q22" s="17"/>
@@ -2054,24 +2045,24 @@
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="61" t="s">
+      <c r="F23" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="60" t="s">
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="P23" s="61" t="s">
+      <c r="P23" s="58" t="s">
         <v>46</v>
       </c>
       <c r="Q23" s="13"/>
@@ -2135,7 +2126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4C9B7A-925E-4ACB-8F3D-3CC4DA199EDA}">
   <dimension ref="B2:AP28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AI31" sqref="AI31"/>
     </sheetView>
   </sheetViews>
@@ -2150,45 +2141,45 @@
   <sheetData>
     <row r="2" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="2:42" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="80"/>
-      <c r="M3" s="78" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="74"/>
+      <c r="M3" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
-      <c r="T3" s="79"/>
-      <c r="U3" s="79"/>
-      <c r="V3" s="79"/>
-      <c r="W3" s="79"/>
-      <c r="X3" s="79"/>
-      <c r="Y3" s="79"/>
-      <c r="Z3" s="80"/>
-      <c r="AB3" s="78" t="s">
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="73"/>
+      <c r="V3" s="73"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
+      <c r="Y3" s="73"/>
+      <c r="Z3" s="74"/>
+      <c r="AB3" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="AC3" s="79"/>
-      <c r="AD3" s="79"/>
-      <c r="AE3" s="79"/>
-      <c r="AF3" s="79"/>
-      <c r="AG3" s="79"/>
-      <c r="AH3" s="79"/>
-      <c r="AI3" s="79"/>
-      <c r="AJ3" s="80"/>
+      <c r="AC3" s="73"/>
+      <c r="AD3" s="73"/>
+      <c r="AE3" s="73"/>
+      <c r="AF3" s="73"/>
+      <c r="AG3" s="73"/>
+      <c r="AH3" s="73"/>
+      <c r="AI3" s="73"/>
+      <c r="AJ3" s="74"/>
       <c r="AK3" s="42"/>
       <c r="AL3" s="42"/>
       <c r="AM3" s="42"/>
@@ -2239,12 +2230,12 @@
       <c r="D5" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
       <c r="I5" s="24" t="s">
         <v>59</v>
       </c>
@@ -2256,16 +2247,16 @@
       <c r="O5" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="84" t="s">
+      <c r="P5" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="84"/>
-      <c r="S5" s="84"/>
-      <c r="T5" s="84"/>
-      <c r="U5" s="84"/>
-      <c r="V5" s="84"/>
-      <c r="W5" s="84"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78"/>
+      <c r="T5" s="78"/>
+      <c r="U5" s="78"/>
+      <c r="V5" s="78"/>
+      <c r="W5" s="78"/>
       <c r="X5" s="35" t="s">
         <v>78</v>
       </c>
@@ -2280,11 +2271,11 @@
       <c r="AD5" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="AE5" s="81" t="s">
+      <c r="AE5" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="AF5" s="81"/>
-      <c r="AG5" s="81"/>
+      <c r="AF5" s="75"/>
+      <c r="AG5" s="75"/>
       <c r="AH5" s="44" t="s">
         <v>95</v>
       </c>
@@ -2301,32 +2292,32 @@
       <c r="D6" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
       <c r="I6" s="25" t="s">
         <v>60</v>
       </c>
       <c r="K6" s="5"/>
       <c r="M6" s="4"/>
       <c r="O6" s="36"/>
-      <c r="P6" s="85"/>
-      <c r="Q6" s="85"/>
-      <c r="R6" s="85"/>
-      <c r="S6" s="85"/>
-      <c r="T6" s="85"/>
-      <c r="U6" s="85"/>
-      <c r="V6" s="85"/>
-      <c r="W6" s="85"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
       <c r="X6" s="37"/>
       <c r="Z6" s="5"/>
       <c r="AB6" s="4"/>
       <c r="AC6" s="51"/>
       <c r="AD6" s="45"/>
-      <c r="AE6" s="82"/>
-      <c r="AF6" s="82"/>
-      <c r="AG6" s="82"/>
+      <c r="AE6" s="76"/>
+      <c r="AF6" s="76"/>
+      <c r="AG6" s="76"/>
       <c r="AH6" s="46"/>
       <c r="AI6" s="50"/>
       <c r="AJ6" s="5"/>
@@ -2334,10 +2325,10 @@
     <row r="7" spans="2:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
       <c r="I7" s="5"/>
       <c r="K7" s="5"/>
       <c r="M7" s="4"/>
@@ -2347,14 +2338,14 @@
       <c r="O7" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P7" s="86"/>
-      <c r="Q7" s="86"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="86"/>
-      <c r="T7" s="86"/>
-      <c r="U7" s="86"/>
-      <c r="V7" s="86"/>
-      <c r="W7" s="86"/>
+      <c r="P7" s="80"/>
+      <c r="Q7" s="80"/>
+      <c r="R7" s="80"/>
+      <c r="S7" s="80"/>
+      <c r="T7" s="80"/>
+      <c r="U7" s="80"/>
+      <c r="V7" s="80"/>
+      <c r="W7" s="80"/>
       <c r="X7" s="39" t="s">
         <v>79</v>
       </c>
@@ -2369,9 +2360,9 @@
       <c r="AD7" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="AE7" s="83"/>
-      <c r="AF7" s="83"/>
-      <c r="AG7" s="83"/>
+      <c r="AE7" s="77"/>
+      <c r="AF7" s="77"/>
+      <c r="AG7" s="77"/>
       <c r="AH7" s="48" t="s">
         <v>96</v>
       </c>
@@ -2388,10 +2379,10 @@
       <c r="D8" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
       <c r="I8" s="26" t="s">
         <v>61</v>
       </c>
@@ -2412,10 +2403,10 @@
       <c r="D9" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
       <c r="I9" s="27" t="s">
         <v>62</v>
       </c>
@@ -2430,16 +2421,16 @@
       <c r="O9" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P9" s="84" t="s">
+      <c r="P9" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="Q9" s="84"/>
-      <c r="R9" s="84"/>
-      <c r="S9" s="84"/>
-      <c r="T9" s="84"/>
-      <c r="U9" s="84"/>
-      <c r="V9" s="84"/>
-      <c r="W9" s="84"/>
+      <c r="Q9" s="78"/>
+      <c r="R9" s="78"/>
+      <c r="S9" s="78"/>
+      <c r="T9" s="78"/>
+      <c r="U9" s="78"/>
+      <c r="V9" s="78"/>
+      <c r="W9" s="78"/>
       <c r="X9" s="35" t="s">
         <v>78</v>
       </c>
@@ -2455,14 +2446,14 @@
       <c r="K10" s="5"/>
       <c r="M10" s="4"/>
       <c r="O10" s="36"/>
-      <c r="P10" s="85"/>
-      <c r="Q10" s="85"/>
-      <c r="R10" s="85"/>
-      <c r="S10" s="85"/>
-      <c r="T10" s="85"/>
-      <c r="U10" s="85"/>
-      <c r="V10" s="85"/>
-      <c r="W10" s="85"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="79"/>
+      <c r="T10" s="79"/>
+      <c r="U10" s="79"/>
+      <c r="V10" s="79"/>
+      <c r="W10" s="79"/>
       <c r="X10" s="37"/>
       <c r="Z10" s="5"/>
       <c r="AB10" s="4"/>
@@ -2476,12 +2467,12 @@
       <c r="D11" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
       <c r="I11" s="24" t="s">
         <v>59</v>
       </c>
@@ -2493,14 +2484,14 @@
       <c r="O11" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="86"/>
-      <c r="R11" s="86"/>
-      <c r="S11" s="86"/>
-      <c r="T11" s="86"/>
-      <c r="U11" s="86"/>
-      <c r="V11" s="86"/>
-      <c r="W11" s="86"/>
+      <c r="P11" s="80"/>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="80"/>
+      <c r="S11" s="80"/>
+      <c r="T11" s="80"/>
+      <c r="U11" s="80"/>
+      <c r="V11" s="80"/>
+      <c r="W11" s="80"/>
       <c r="X11" s="39" t="s">
         <v>79</v>
       </c>
@@ -2519,10 +2510,10 @@
       <c r="D12" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
       <c r="I12" s="25" t="s">
         <v>60</v>
       </c>
@@ -2535,10 +2526,10 @@
     <row r="13" spans="2:42" x14ac:dyDescent="0.45">
       <c r="B13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="76"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
       <c r="I13" s="5"/>
       <c r="K13" s="5"/>
       <c r="M13" s="4"/>
@@ -2548,16 +2539,16 @@
       <c r="O13" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P13" s="84" t="s">
+      <c r="P13" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="Q13" s="84"/>
-      <c r="R13" s="84"/>
-      <c r="S13" s="84"/>
-      <c r="T13" s="84"/>
-      <c r="U13" s="84"/>
-      <c r="V13" s="84"/>
-      <c r="W13" s="84"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="78"/>
+      <c r="S13" s="78"/>
+      <c r="T13" s="78"/>
+      <c r="U13" s="78"/>
+      <c r="V13" s="78"/>
+      <c r="W13" s="78"/>
       <c r="X13" s="35" t="s">
         <v>78</v>
       </c>
@@ -2576,10 +2567,10 @@
       <c r="D14" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
       <c r="I14" s="26" t="s">
         <v>61</v>
       </c>
@@ -2589,14 +2580,14 @@
       <c r="K14" s="5"/>
       <c r="M14" s="4"/>
       <c r="O14" s="36"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="85"/>
-      <c r="V14" s="85"/>
-      <c r="W14" s="85"/>
+      <c r="P14" s="79"/>
+      <c r="Q14" s="79"/>
+      <c r="R14" s="79"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="79"/>
+      <c r="U14" s="79"/>
+      <c r="V14" s="79"/>
+      <c r="W14" s="79"/>
       <c r="X14" s="37"/>
       <c r="Z14" s="5"/>
       <c r="AB14" s="4"/>
@@ -2610,10 +2601,10 @@
       <c r="D15" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71"/>
       <c r="I15" s="27" t="s">
         <v>62</v>
       </c>
@@ -2628,14 +2619,14 @@
       <c r="O15" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P15" s="86"/>
-      <c r="Q15" s="86"/>
-      <c r="R15" s="86"/>
-      <c r="S15" s="86"/>
-      <c r="T15" s="86"/>
-      <c r="U15" s="86"/>
-      <c r="V15" s="86"/>
-      <c r="W15" s="86"/>
+      <c r="P15" s="80"/>
+      <c r="Q15" s="80"/>
+      <c r="R15" s="80"/>
+      <c r="S15" s="80"/>
+      <c r="T15" s="80"/>
+      <c r="U15" s="80"/>
+      <c r="V15" s="80"/>
+      <c r="W15" s="80"/>
       <c r="X15" s="39" t="s">
         <v>79</v>
       </c>
@@ -2669,12 +2660,12 @@
       <c r="D17" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="75" t="s">
+      <c r="E17" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
       <c r="I17" s="24" t="s">
         <v>59</v>
       </c>
@@ -2686,16 +2677,16 @@
       <c r="O17" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P17" s="84" t="s">
+      <c r="P17" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="Q17" s="84"/>
-      <c r="R17" s="84"/>
-      <c r="S17" s="84"/>
-      <c r="T17" s="84"/>
-      <c r="U17" s="84"/>
-      <c r="V17" s="84"/>
-      <c r="W17" s="84"/>
+      <c r="Q17" s="78"/>
+      <c r="R17" s="78"/>
+      <c r="S17" s="78"/>
+      <c r="T17" s="78"/>
+      <c r="U17" s="78"/>
+      <c r="V17" s="78"/>
+      <c r="W17" s="78"/>
       <c r="X17" s="35" t="s">
         <v>78</v>
       </c>
@@ -2712,45 +2703,45 @@
       <c r="D18" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
       <c r="I18" s="25" t="s">
         <v>60</v>
       </c>
       <c r="K18" s="5"/>
       <c r="M18" s="4"/>
       <c r="O18" s="36"/>
-      <c r="P18" s="85"/>
-      <c r="Q18" s="85"/>
-      <c r="R18" s="85"/>
-      <c r="S18" s="85"/>
-      <c r="T18" s="85"/>
-      <c r="U18" s="85"/>
-      <c r="V18" s="85"/>
-      <c r="W18" s="85"/>
+      <c r="P18" s="79"/>
+      <c r="Q18" s="79"/>
+      <c r="R18" s="79"/>
+      <c r="S18" s="79"/>
+      <c r="T18" s="79"/>
+      <c r="U18" s="79"/>
+      <c r="V18" s="79"/>
+      <c r="W18" s="79"/>
       <c r="X18" s="37"/>
       <c r="Z18" s="5"/>
-      <c r="AB18" s="78" t="s">
+      <c r="AB18" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="AC18" s="79"/>
-      <c r="AD18" s="79"/>
-      <c r="AE18" s="79"/>
-      <c r="AF18" s="79"/>
-      <c r="AG18" s="79"/>
-      <c r="AH18" s="79"/>
-      <c r="AI18" s="79"/>
-      <c r="AJ18" s="80"/>
+      <c r="AC18" s="73"/>
+      <c r="AD18" s="73"/>
+      <c r="AE18" s="73"/>
+      <c r="AF18" s="73"/>
+      <c r="AG18" s="73"/>
+      <c r="AH18" s="73"/>
+      <c r="AI18" s="73"/>
+      <c r="AJ18" s="74"/>
     </row>
     <row r="19" spans="2:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="76"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
       <c r="I19" s="5"/>
       <c r="K19" s="5"/>
       <c r="M19" s="4"/>
@@ -2760,14 +2751,14 @@
       <c r="O19" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P19" s="86"/>
-      <c r="Q19" s="86"/>
-      <c r="R19" s="86"/>
-      <c r="S19" s="86"/>
-      <c r="T19" s="86"/>
-      <c r="U19" s="86"/>
-      <c r="V19" s="86"/>
-      <c r="W19" s="86"/>
+      <c r="P19" s="80"/>
+      <c r="Q19" s="80"/>
+      <c r="R19" s="80"/>
+      <c r="S19" s="80"/>
+      <c r="T19" s="80"/>
+      <c r="U19" s="80"/>
+      <c r="V19" s="80"/>
+      <c r="W19" s="80"/>
       <c r="X19" s="39" t="s">
         <v>79</v>
       </c>
@@ -2793,10 +2784,10 @@
       <c r="D20" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
       <c r="I20" s="26" t="s">
         <v>61</v>
       </c>
@@ -2813,11 +2804,11 @@
       <c r="AD20" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="AE20" s="81" t="s">
+      <c r="AE20" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="AF20" s="81"/>
-      <c r="AG20" s="81"/>
+      <c r="AF20" s="75"/>
+      <c r="AG20" s="75"/>
       <c r="AH20" s="3"/>
       <c r="AJ20" s="5"/>
     </row>
@@ -2829,10 +2820,10 @@
       <c r="D21" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="77"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
       <c r="I21" s="27" t="s">
         <v>62</v>
       </c>
@@ -2845,9 +2836,9 @@
       <c r="AB21" s="4"/>
       <c r="AC21" s="51"/>
       <c r="AD21" s="45"/>
-      <c r="AE21" s="82"/>
-      <c r="AF21" s="82"/>
-      <c r="AG21" s="82"/>
+      <c r="AE21" s="76"/>
+      <c r="AF21" s="76"/>
+      <c r="AG21" s="76"/>
       <c r="AH21" s="53" t="s">
         <v>99</v>
       </c>
@@ -2868,9 +2859,9 @@
       <c r="AD22" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="AE22" s="83"/>
-      <c r="AF22" s="83"/>
-      <c r="AG22" s="83"/>
+      <c r="AE22" s="77"/>
+      <c r="AF22" s="77"/>
+      <c r="AG22" s="77"/>
       <c r="AH22" s="8"/>
       <c r="AJ22" s="5"/>
     </row>
@@ -2882,12 +2873,12 @@
       <c r="D23" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="75" t="s">
+      <c r="E23" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="75"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
       <c r="I23" s="24" t="s">
         <v>59</v>
       </c>
@@ -2905,10 +2896,10 @@
       <c r="D24" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="76"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
       <c r="I24" s="25" t="s">
         <v>60</v>
       </c>
@@ -2922,21 +2913,21 @@
       <c r="AD24" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="AE24" s="81" t="s">
+      <c r="AE24" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="AF24" s="81"/>
-      <c r="AG24" s="81"/>
+      <c r="AF24" s="75"/>
+      <c r="AG24" s="75"/>
       <c r="AH24" s="3"/>
       <c r="AJ24" s="5"/>
     </row>
     <row r="25" spans="2:36" ht="19.5" x14ac:dyDescent="0.6">
       <c r="B25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="76"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
       <c r="I25" s="5"/>
       <c r="K25" s="5"/>
       <c r="M25" s="4"/>
@@ -2944,9 +2935,9 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="51"/>
       <c r="AD25" s="45"/>
-      <c r="AE25" s="82"/>
-      <c r="AF25" s="82"/>
-      <c r="AG25" s="82"/>
+      <c r="AE25" s="76"/>
+      <c r="AF25" s="76"/>
+      <c r="AG25" s="76"/>
       <c r="AH25" s="53" t="s">
         <v>99</v>
       </c>
@@ -2963,10 +2954,10 @@
       <c r="D26" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="76"/>
-      <c r="F26" s="76"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="76"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
       <c r="I26" s="26" t="s">
         <v>61</v>
       </c>
@@ -2983,9 +2974,9 @@
       <c r="AD26" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="AE26" s="83"/>
-      <c r="AF26" s="83"/>
-      <c r="AG26" s="83"/>
+      <c r="AE26" s="77"/>
+      <c r="AF26" s="77"/>
+      <c r="AG26" s="77"/>
       <c r="AH26" s="8"/>
       <c r="AJ26" s="5"/>
     </row>
@@ -2997,10 +2988,10 @@
       <c r="D27" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="77"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="77"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
       <c r="I27" s="27" t="s">
         <v>62</v>
       </c>

</xml_diff>